<commit_message>
fikset småting i excel ark
</commit_message>
<xml_diff>
--- a/docs/adr/0001-API-FSS.xlsx
+++ b/docs/adr/0001-API-FSS.xlsx
@@ -95,9 +95,6 @@
     <t>beholdes som den er</t>
   </si>
   <si>
-    <t>beholdes i fss, sbs kan kalle tjenesten</t>
-  </si>
-  <si>
     <t xml:space="preserve">her er det ifsetninger som skiller hva som skal kjøres ut ifra sone, koden må splittes </t>
   </si>
   <si>
@@ -114,6 +111,9 @@
   </si>
   <si>
     <t>Ansvaret til applikasjonen er å ta imot kall fra saksbehandling frontend. Noen tjenester tilbyr den selv sånn som S3 og whitelisting. De fleste andre tjeneste tilbys av nav registre og andre tjenester</t>
+  </si>
+  <si>
+    <t>Inneholder to metoder, en kjøres i SBS en kjøres i FSS</t>
   </si>
 </sst>
 </file>
@@ -451,12 +451,12 @@
   <dimension ref="A1:D26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="105.28515625" customWidth="1"/>
+    <col min="1" max="1" width="45" customWidth="1"/>
     <col min="2" max="2" width="121" style="4" customWidth="1"/>
     <col min="3" max="3" width="34.140625" customWidth="1"/>
   </cols>
@@ -488,7 +488,7 @@
       </c>
       <c r="B4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -504,7 +504,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -520,7 +520,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -553,12 +553,7 @@
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>22</v>
-      </c>
+      <c r="B13" s="5"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
@@ -571,7 +566,7 @@
         <v>10</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -587,7 +582,7 @@
         <v>12</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -595,7 +590,7 @@
         <v>14</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -603,7 +598,15 @@
         <v>15</v>
       </c>
       <c r="B19" s="5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>24</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -613,18 +616,18 @@
     </row>
     <row r="25" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>